<commit_message>
add faq.xlsx for deployment
</commit_message>
<xml_diff>
--- a/faq.xlsx
+++ b/faq.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Tạo Chatbot AI_v3\chatbox-support-corrected\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D21CC90-A46A-4C36-A7D8-70427869EE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B884A9AA-8970-42F7-A86D-1A780A16979B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>question</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>Cấu hình storm control được sử dụng để giới hạn các bản tin broadcast,multicast,unknown unicast. Có thể bảo vệ mạng khỏi các cơn bão lưu lượng truy cập bằng cách đặt ngưỡng cho lưu lượng truy cập broadcast, multicast hoặc unknown unicast. Bất kỳ gói nào vượt quá ngưỡng quy định sau đó sẽ bị loại bỏ.</t>
+  </si>
+  <si>
+    <t>Cấu hình Vlan Switch HPE1111</t>
+  </si>
+  <si>
+    <t>Cấu hình Vlan Switch UPE5523</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>cdf</t>
   </si>
 </sst>
 </file>
@@ -457,9 +469,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -517,33 +531,49 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>